<commit_message>
Added support for few more texts
</commit_message>
<xml_diff>
--- a/docs/Queries_CCG_Derivation.xlsx
+++ b/docs/Queries_CCG_Derivation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="CCG" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="67">
   <si>
     <t xml:space="preserve">What</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">(S\NP)\T)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(S\T)</t>
   </si>
   <si>
     <t xml:space="preserve">Tasks</t>
@@ -1247,7 +1250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1269,6 +1272,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1361,10 +1368,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:R75"/>
+  <dimension ref="B2:R82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E77" activeCellId="0" sqref="E77"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B82" activeCellId="0" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1986,8 +1993,30 @@
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
     </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="38">
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="F7:I7"/>
@@ -2025,6 +2054,7 @@
     <mergeCell ref="F73:I73"/>
     <mergeCell ref="B74:E74"/>
     <mergeCell ref="B75:I75"/>
+    <mergeCell ref="B82:C82"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2043,8 +2073,8 @@
   </sheetPr>
   <dimension ref="B1:B33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2055,166 +2085,166 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="6" t="s">
-        <v>34</v>
+      <c r="B1" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="6"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="7" t="s">
-        <v>60</v>
+      <c r="B29" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2245,8 +2275,8 @@
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="259.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="8" t="s">
-        <v>65</v>
+      <c r="D5" s="9" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>